<commit_message>
Atualizado por script em 10-11-2023 02:45
</commit_message>
<xml_diff>
--- a/2023/romania_liga-2_2023-2024.xlsx
+++ b/2023/romania_liga-2_2023-2024.xlsx
@@ -429,7 +429,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:V121"/>
+  <dimension ref="A1:V122"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1401,22 +1401,22 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>Unirea Slobozia</t>
+          <t>Selimbar</t>
         </is>
       </c>
       <c r="G11" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="H11" t="inlineStr">
         <is>
-          <t>Viitorul Tg. Jiu</t>
+          <t>Unirea Dej</t>
         </is>
       </c>
       <c r="I11" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J11" t="n">
-        <v>1.58</v>
+        <v>2.06</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
@@ -1424,15 +1424,15 @@
         </is>
       </c>
       <c r="L11" t="n">
-        <v>1.49</v>
+        <v>2.2</v>
       </c>
       <c r="M11" t="inlineStr">
         <is>
-          <t>12/08/2023 09:14</t>
+          <t>12/08/2023 09:56</t>
         </is>
       </c>
       <c r="N11" t="n">
-        <v>3.77</v>
+        <v>3</v>
       </c>
       <c r="O11" t="inlineStr">
         <is>
@@ -1440,15 +1440,15 @@
         </is>
       </c>
       <c r="P11" t="n">
-        <v>4.35</v>
+        <v>2.98</v>
       </c>
       <c r="Q11" t="inlineStr">
         <is>
-          <t>12/08/2023 09:14</t>
+          <t>12/08/2023 09:56</t>
         </is>
       </c>
       <c r="R11" t="n">
-        <v>5.17</v>
+        <v>3.52</v>
       </c>
       <c r="S11" t="inlineStr">
         <is>
@@ -1456,16 +1456,16 @@
         </is>
       </c>
       <c r="T11" t="n">
-        <v>6.51</v>
+        <v>3.73</v>
       </c>
       <c r="U11" t="inlineStr">
         <is>
-          <t>12/08/2023 09:14</t>
+          <t>12/08/2023 09:56</t>
         </is>
       </c>
       <c r="V11" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/romania/liga-2/unirea-slobozia-viitorul-targu-jiu/rwLG2m1j/</t>
+          <t>https://www.betexplorer.com/football/romania/liga-2/selimbar-unirea-dej/OYyYABgA/</t>
         </is>
       </c>
     </row>
@@ -1861,22 +1861,22 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>Selimbar</t>
+          <t>Unirea Slobozia</t>
         </is>
       </c>
       <c r="G16" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H16" t="inlineStr">
         <is>
-          <t>Unirea Dej</t>
+          <t>Viitorul Tg. Jiu</t>
         </is>
       </c>
       <c r="I16" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J16" t="n">
-        <v>2.06</v>
+        <v>1.58</v>
       </c>
       <c r="K16" t="inlineStr">
         <is>
@@ -1884,15 +1884,15 @@
         </is>
       </c>
       <c r="L16" t="n">
-        <v>2.2</v>
+        <v>1.49</v>
       </c>
       <c r="M16" t="inlineStr">
         <is>
-          <t>12/08/2023 09:56</t>
+          <t>12/08/2023 09:14</t>
         </is>
       </c>
       <c r="N16" t="n">
-        <v>3</v>
+        <v>3.77</v>
       </c>
       <c r="O16" t="inlineStr">
         <is>
@@ -1900,15 +1900,15 @@
         </is>
       </c>
       <c r="P16" t="n">
-        <v>2.98</v>
+        <v>4.35</v>
       </c>
       <c r="Q16" t="inlineStr">
         <is>
-          <t>12/08/2023 09:56</t>
+          <t>12/08/2023 09:14</t>
         </is>
       </c>
       <c r="R16" t="n">
-        <v>3.52</v>
+        <v>5.17</v>
       </c>
       <c r="S16" t="inlineStr">
         <is>
@@ -1916,16 +1916,16 @@
         </is>
       </c>
       <c r="T16" t="n">
-        <v>3.73</v>
+        <v>6.51</v>
       </c>
       <c r="U16" t="inlineStr">
         <is>
-          <t>12/08/2023 09:56</t>
+          <t>12/08/2023 09:14</t>
         </is>
       </c>
       <c r="V16" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/romania/liga-2/selimbar-unirea-dej/OYyYABgA/</t>
+          <t>https://www.betexplorer.com/football/romania/liga-2/unirea-slobozia-viitorul-targu-jiu/rwLG2m1j/</t>
         </is>
       </c>
     </row>
@@ -8025,71 +8025,71 @@
       </c>
       <c r="F83" t="inlineStr">
         <is>
-          <t>Chindia Targoviste</t>
+          <t>Viitorul Tg. Jiu</t>
         </is>
       </c>
       <c r="G83" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H83" t="inlineStr">
         <is>
-          <t>Progresul Spartac</t>
+          <t>Concordia</t>
         </is>
       </c>
       <c r="I83" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="J83" t="n">
-        <v>1.2</v>
+        <v>4.16</v>
       </c>
       <c r="K83" t="inlineStr">
         <is>
-          <t>07/10/2023 00:13</t>
+          <t>05/10/2023 21:13</t>
         </is>
       </c>
       <c r="L83" t="n">
-        <v>1.17</v>
+        <v>5.13</v>
       </c>
       <c r="M83" t="inlineStr">
         <is>
-          <t>07/10/2023 08:28</t>
+          <t>07/10/2023 09:52</t>
         </is>
       </c>
       <c r="N83" t="n">
-        <v>6.4</v>
+        <v>3.41</v>
       </c>
       <c r="O83" t="inlineStr">
         <is>
-          <t>07/10/2023 00:13</t>
+          <t>05/10/2023 21:13</t>
         </is>
       </c>
       <c r="P83" t="n">
-        <v>7.19</v>
+        <v>3.55</v>
       </c>
       <c r="Q83" t="inlineStr">
         <is>
-          <t>07/10/2023 09:33</t>
+          <t>07/10/2023 09:52</t>
         </is>
       </c>
       <c r="R83" t="n">
-        <v>12.64</v>
+        <v>1.76</v>
       </c>
       <c r="S83" t="inlineStr">
         <is>
-          <t>07/10/2023 00:13</t>
+          <t>05/10/2023 21:13</t>
         </is>
       </c>
       <c r="T83" t="n">
-        <v>16.45</v>
+        <v>1.72</v>
       </c>
       <c r="U83" t="inlineStr">
         <is>
-          <t>07/10/2023 09:33</t>
+          <t>07/10/2023 09:52</t>
         </is>
       </c>
       <c r="V83" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/romania/liga-2/chindia-targoviste-progresul-spartac/0xz9njTr/</t>
+          <t>https://www.betexplorer.com/football/romania/liga-2/viitorul-targu-jiu-concordia/21fYhhjF/</t>
         </is>
       </c>
     </row>
@@ -8117,22 +8117,22 @@
       </c>
       <c r="F84" t="inlineStr">
         <is>
-          <t>Alexandria</t>
+          <t>Unirea Dej</t>
         </is>
       </c>
       <c r="G84" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H84" t="inlineStr">
         <is>
-          <t>Ceahlaul</t>
+          <t>CSC Dumbravita</t>
         </is>
       </c>
       <c r="I84" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J84" t="n">
-        <v>3.31</v>
+        <v>2.17</v>
       </c>
       <c r="K84" t="inlineStr">
         <is>
@@ -8140,15 +8140,15 @@
         </is>
       </c>
       <c r="L84" t="n">
-        <v>3.37</v>
+        <v>2.41</v>
       </c>
       <c r="M84" t="inlineStr">
         <is>
-          <t>07/10/2023 09:53</t>
+          <t>07/10/2023 09:44</t>
         </is>
       </c>
       <c r="N84" t="n">
-        <v>3.06</v>
+        <v>3.2</v>
       </c>
       <c r="O84" t="inlineStr">
         <is>
@@ -8156,15 +8156,15 @@
         </is>
       </c>
       <c r="P84" t="n">
-        <v>3.19</v>
+        <v>3.14</v>
       </c>
       <c r="Q84" t="inlineStr">
         <is>
-          <t>07/10/2023 09:36</t>
+          <t>07/10/2023 09:43</t>
         </is>
       </c>
       <c r="R84" t="n">
-        <v>2.12</v>
+        <v>3.04</v>
       </c>
       <c r="S84" t="inlineStr">
         <is>
@@ -8172,16 +8172,16 @@
         </is>
       </c>
       <c r="T84" t="n">
-        <v>2.24</v>
+        <v>3.08</v>
       </c>
       <c r="U84" t="inlineStr">
         <is>
-          <t>07/10/2023 09:53</t>
+          <t>07/10/2023 09:44</t>
         </is>
       </c>
       <c r="V84" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/romania/liga-2/csm-alexandria-ceahlaul/z9sLqlD1/</t>
+          <t>https://www.betexplorer.com/football/romania/liga-2/unirea-dej-csc-dumbravita/hphGpUce/</t>
         </is>
       </c>
     </row>
@@ -8209,22 +8209,22 @@
       </c>
       <c r="F85" t="inlineStr">
         <is>
-          <t>Metaloglobus Bucharest</t>
+          <t>Mioveni</t>
         </is>
       </c>
       <c r="G85" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="H85" t="inlineStr">
         <is>
-          <t>Csikszereda M. Ciuc</t>
+          <t>CSM Resita</t>
         </is>
       </c>
       <c r="I85" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J85" t="n">
-        <v>2.48</v>
+        <v>1.75</v>
       </c>
       <c r="K85" t="inlineStr">
         <is>
@@ -8232,15 +8232,15 @@
         </is>
       </c>
       <c r="L85" t="n">
-        <v>2.46</v>
+        <v>1.81</v>
       </c>
       <c r="M85" t="inlineStr">
         <is>
-          <t>07/10/2023 09:57</t>
+          <t>07/10/2023 09:51</t>
         </is>
       </c>
       <c r="N85" t="n">
-        <v>2.95</v>
+        <v>3.38</v>
       </c>
       <c r="O85" t="inlineStr">
         <is>
@@ -8248,15 +8248,15 @@
         </is>
       </c>
       <c r="P85" t="n">
-        <v>3.13</v>
+        <v>3.47</v>
       </c>
       <c r="Q85" t="inlineStr">
         <is>
-          <t>07/10/2023 09:57</t>
+          <t>07/10/2023 09:51</t>
         </is>
       </c>
       <c r="R85" t="n">
-        <v>2.79</v>
+        <v>4.26</v>
       </c>
       <c r="S85" t="inlineStr">
         <is>
@@ -8264,16 +8264,16 @@
         </is>
       </c>
       <c r="T85" t="n">
-        <v>3.03</v>
+        <v>4.59</v>
       </c>
       <c r="U85" t="inlineStr">
         <is>
-          <t>07/10/2023 09:57</t>
+          <t>07/10/2023 09:51</t>
         </is>
       </c>
       <c r="V85" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/romania/liga-2/metaloglobus-bucharest-miercurea-ciuc/faZCoArk/</t>
+          <t>https://www.betexplorer.com/football/romania/liga-2/mioveni-csm-resita/thgxhC5L/</t>
         </is>
       </c>
     </row>
@@ -8301,7 +8301,7 @@
       </c>
       <c r="F86" t="inlineStr">
         <is>
-          <t>Mioveni</t>
+          <t>Alexandria</t>
         </is>
       </c>
       <c r="G86" t="n">
@@ -8309,14 +8309,14 @@
       </c>
       <c r="H86" t="inlineStr">
         <is>
-          <t>CSM Resita</t>
+          <t>Ceahlaul</t>
         </is>
       </c>
       <c r="I86" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J86" t="n">
-        <v>1.75</v>
+        <v>3.31</v>
       </c>
       <c r="K86" t="inlineStr">
         <is>
@@ -8324,15 +8324,15 @@
         </is>
       </c>
       <c r="L86" t="n">
-        <v>1.81</v>
+        <v>3.37</v>
       </c>
       <c r="M86" t="inlineStr">
         <is>
-          <t>07/10/2023 09:51</t>
+          <t>07/10/2023 09:53</t>
         </is>
       </c>
       <c r="N86" t="n">
-        <v>3.38</v>
+        <v>3.06</v>
       </c>
       <c r="O86" t="inlineStr">
         <is>
@@ -8340,15 +8340,15 @@
         </is>
       </c>
       <c r="P86" t="n">
-        <v>3.47</v>
+        <v>3.19</v>
       </c>
       <c r="Q86" t="inlineStr">
         <is>
-          <t>07/10/2023 09:51</t>
+          <t>07/10/2023 09:36</t>
         </is>
       </c>
       <c r="R86" t="n">
-        <v>4.26</v>
+        <v>2.12</v>
       </c>
       <c r="S86" t="inlineStr">
         <is>
@@ -8356,16 +8356,16 @@
         </is>
       </c>
       <c r="T86" t="n">
-        <v>4.59</v>
+        <v>2.24</v>
       </c>
       <c r="U86" t="inlineStr">
         <is>
-          <t>07/10/2023 09:51</t>
+          <t>07/10/2023 09:53</t>
         </is>
       </c>
       <c r="V86" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/romania/liga-2/mioveni-csm-resita/thgxhC5L/</t>
+          <t>https://www.betexplorer.com/football/romania/liga-2/csm-alexandria-ceahlaul/z9sLqlD1/</t>
         </is>
       </c>
     </row>
@@ -8393,71 +8393,71 @@
       </c>
       <c r="F87" t="inlineStr">
         <is>
-          <t>Unirea Dej</t>
+          <t>Chindia Targoviste</t>
         </is>
       </c>
       <c r="G87" t="n">
+        <v>3</v>
+      </c>
+      <c r="H87" t="inlineStr">
+        <is>
+          <t>Progresul Spartac</t>
+        </is>
+      </c>
+      <c r="I87" t="n">
         <v>0</v>
       </c>
-      <c r="H87" t="inlineStr">
-        <is>
-          <t>CSC Dumbravita</t>
-        </is>
-      </c>
-      <c r="I87" t="n">
-        <v>1</v>
-      </c>
       <c r="J87" t="n">
-        <v>2.17</v>
+        <v>1.2</v>
       </c>
       <c r="K87" t="inlineStr">
         <is>
-          <t>05/10/2023 21:13</t>
+          <t>07/10/2023 00:13</t>
         </is>
       </c>
       <c r="L87" t="n">
-        <v>2.41</v>
+        <v>1.17</v>
       </c>
       <c r="M87" t="inlineStr">
         <is>
-          <t>07/10/2023 09:44</t>
+          <t>07/10/2023 08:28</t>
         </is>
       </c>
       <c r="N87" t="n">
-        <v>3.2</v>
+        <v>6.4</v>
       </c>
       <c r="O87" t="inlineStr">
         <is>
-          <t>05/10/2023 21:13</t>
+          <t>07/10/2023 00:13</t>
         </is>
       </c>
       <c r="P87" t="n">
-        <v>3.14</v>
+        <v>7.19</v>
       </c>
       <c r="Q87" t="inlineStr">
         <is>
-          <t>07/10/2023 09:43</t>
+          <t>07/10/2023 09:33</t>
         </is>
       </c>
       <c r="R87" t="n">
-        <v>3.04</v>
+        <v>12.64</v>
       </c>
       <c r="S87" t="inlineStr">
         <is>
-          <t>05/10/2023 21:13</t>
+          <t>07/10/2023 00:13</t>
         </is>
       </c>
       <c r="T87" t="n">
-        <v>3.08</v>
+        <v>16.45</v>
       </c>
       <c r="U87" t="inlineStr">
         <is>
-          <t>07/10/2023 09:44</t>
+          <t>07/10/2023 09:33</t>
         </is>
       </c>
       <c r="V87" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/romania/liga-2/unirea-dej-csc-dumbravita/hphGpUce/</t>
+          <t>https://www.betexplorer.com/football/romania/liga-2/chindia-targoviste-progresul-spartac/0xz9njTr/</t>
         </is>
       </c>
     </row>
@@ -8485,22 +8485,22 @@
       </c>
       <c r="F88" t="inlineStr">
         <is>
-          <t>Viitorul Tg. Jiu</t>
+          <t>Metaloglobus Bucharest</t>
         </is>
       </c>
       <c r="G88" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="H88" t="inlineStr">
         <is>
-          <t>Concordia</t>
+          <t>Csikszereda M. Ciuc</t>
         </is>
       </c>
       <c r="I88" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="J88" t="n">
-        <v>4.16</v>
+        <v>2.48</v>
       </c>
       <c r="K88" t="inlineStr">
         <is>
@@ -8508,15 +8508,15 @@
         </is>
       </c>
       <c r="L88" t="n">
-        <v>5.13</v>
+        <v>2.46</v>
       </c>
       <c r="M88" t="inlineStr">
         <is>
-          <t>07/10/2023 09:52</t>
+          <t>07/10/2023 09:57</t>
         </is>
       </c>
       <c r="N88" t="n">
-        <v>3.41</v>
+        <v>2.95</v>
       </c>
       <c r="O88" t="inlineStr">
         <is>
@@ -8524,15 +8524,15 @@
         </is>
       </c>
       <c r="P88" t="n">
-        <v>3.55</v>
+        <v>3.13</v>
       </c>
       <c r="Q88" t="inlineStr">
         <is>
-          <t>07/10/2023 09:52</t>
+          <t>07/10/2023 09:57</t>
         </is>
       </c>
       <c r="R88" t="n">
-        <v>1.76</v>
+        <v>2.79</v>
       </c>
       <c r="S88" t="inlineStr">
         <is>
@@ -8540,16 +8540,16 @@
         </is>
       </c>
       <c r="T88" t="n">
-        <v>1.72</v>
+        <v>3.03</v>
       </c>
       <c r="U88" t="inlineStr">
         <is>
-          <t>07/10/2023 09:52</t>
+          <t>07/10/2023 09:57</t>
         </is>
       </c>
       <c r="V88" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/romania/liga-2/viitorul-targu-jiu-concordia/21fYhhjF/</t>
+          <t>https://www.betexplorer.com/football/romania/liga-2/metaloglobus-bucharest-miercurea-ciuc/faZCoArk/</t>
         </is>
       </c>
     </row>
@@ -9037,71 +9037,71 @@
       </c>
       <c r="F94" t="inlineStr">
         <is>
-          <t>Progresul Spartac</t>
+          <t>CSC Dumbravita</t>
         </is>
       </c>
       <c r="G94" t="n">
+        <v>2</v>
+      </c>
+      <c r="H94" t="inlineStr">
+        <is>
+          <t>Alexandria</t>
+        </is>
+      </c>
+      <c r="I94" t="n">
         <v>0</v>
       </c>
-      <c r="H94" t="inlineStr">
-        <is>
-          <t>Metaloglobus Bucharest</t>
-        </is>
-      </c>
-      <c r="I94" t="n">
-        <v>1</v>
-      </c>
       <c r="J94" t="n">
-        <v>3.91</v>
+        <v>2.07</v>
       </c>
       <c r="K94" t="inlineStr">
         <is>
-          <t>19/10/2023 21:12</t>
+          <t>20/10/2023 04:42</t>
         </is>
       </c>
       <c r="L94" t="n">
-        <v>5.54</v>
+        <v>2.05</v>
       </c>
       <c r="M94" t="inlineStr">
         <is>
-          <t>21/10/2023 09:58</t>
+          <t>21/10/2023 09:51</t>
         </is>
       </c>
       <c r="N94" t="n">
-        <v>3.34</v>
+        <v>3.2</v>
       </c>
       <c r="O94" t="inlineStr">
         <is>
-          <t>19/10/2023 21:12</t>
+          <t>20/10/2023 04:42</t>
         </is>
       </c>
       <c r="P94" t="n">
-        <v>3.52</v>
+        <v>3.41</v>
       </c>
       <c r="Q94" t="inlineStr">
         <is>
-          <t>21/10/2023 09:58</t>
+          <t>21/10/2023 09:51</t>
         </is>
       </c>
       <c r="R94" t="n">
-        <v>1.83</v>
+        <v>3.38</v>
       </c>
       <c r="S94" t="inlineStr">
         <is>
-          <t>19/10/2023 21:12</t>
+          <t>20/10/2023 04:42</t>
         </is>
       </c>
       <c r="T94" t="n">
-        <v>1.68</v>
+        <v>3.63</v>
       </c>
       <c r="U94" t="inlineStr">
         <is>
-          <t>21/10/2023 09:58</t>
+          <t>21/10/2023 09:51</t>
         </is>
       </c>
       <c r="V94" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/romania/liga-2/progresul-spartac-metaloglobus-bucharest/nTSfdRd7/</t>
+          <t>https://www.betexplorer.com/football/romania/liga-2/csc-dumbravita-csm-alexandria/EFUnbmSf/</t>
         </is>
       </c>
     </row>
@@ -9129,71 +9129,71 @@
       </c>
       <c r="F95" t="inlineStr">
         <is>
-          <t>CSC Dumbravita</t>
+          <t>CSM Resita</t>
         </is>
       </c>
       <c r="G95" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H95" t="inlineStr">
         <is>
-          <t>Alexandria</t>
+          <t>Tunari</t>
         </is>
       </c>
       <c r="I95" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J95" t="n">
-        <v>2.07</v>
+        <v>1.92</v>
       </c>
       <c r="K95" t="inlineStr">
         <is>
-          <t>20/10/2023 04:42</t>
+          <t>19/10/2023 21:12</t>
         </is>
       </c>
       <c r="L95" t="n">
-        <v>2.05</v>
+        <v>1.85</v>
       </c>
       <c r="M95" t="inlineStr">
         <is>
-          <t>21/10/2023 09:51</t>
+          <t>21/10/2023 06:21</t>
         </is>
       </c>
       <c r="N95" t="n">
-        <v>3.2</v>
+        <v>3.35</v>
       </c>
       <c r="O95" t="inlineStr">
         <is>
-          <t>20/10/2023 04:42</t>
+          <t>19/10/2023 21:12</t>
         </is>
       </c>
       <c r="P95" t="n">
-        <v>3.41</v>
+        <v>3.77</v>
       </c>
       <c r="Q95" t="inlineStr">
         <is>
-          <t>21/10/2023 09:51</t>
+          <t>21/10/2023 08:01</t>
         </is>
       </c>
       <c r="R95" t="n">
-        <v>3.38</v>
+        <v>3.54</v>
       </c>
       <c r="S95" t="inlineStr">
         <is>
-          <t>20/10/2023 04:42</t>
+          <t>19/10/2023 21:12</t>
         </is>
       </c>
       <c r="T95" t="n">
-        <v>3.63</v>
+        <v>3.9</v>
       </c>
       <c r="U95" t="inlineStr">
         <is>
-          <t>21/10/2023 09:51</t>
+          <t>21/10/2023 06:21</t>
         </is>
       </c>
       <c r="V95" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/romania/liga-2/csc-dumbravita-csm-alexandria/EFUnbmSf/</t>
+          <t>https://www.betexplorer.com/football/romania/liga-2/csm-resita-tunari/2yBsKUlE/</t>
         </is>
       </c>
     </row>
@@ -9221,22 +9221,22 @@
       </c>
       <c r="F96" t="inlineStr">
         <is>
-          <t>CSM Resita</t>
+          <t>Progresul Spartac</t>
         </is>
       </c>
       <c r="G96" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H96" t="inlineStr">
         <is>
-          <t>Tunari</t>
+          <t>Metaloglobus Bucharest</t>
         </is>
       </c>
       <c r="I96" t="n">
         <v>1</v>
       </c>
       <c r="J96" t="n">
-        <v>1.92</v>
+        <v>3.91</v>
       </c>
       <c r="K96" t="inlineStr">
         <is>
@@ -9244,15 +9244,15 @@
         </is>
       </c>
       <c r="L96" t="n">
-        <v>1.85</v>
+        <v>5.54</v>
       </c>
       <c r="M96" t="inlineStr">
         <is>
-          <t>21/10/2023 06:21</t>
+          <t>21/10/2023 09:58</t>
         </is>
       </c>
       <c r="N96" t="n">
-        <v>3.35</v>
+        <v>3.34</v>
       </c>
       <c r="O96" t="inlineStr">
         <is>
@@ -9260,15 +9260,15 @@
         </is>
       </c>
       <c r="P96" t="n">
-        <v>3.77</v>
+        <v>3.52</v>
       </c>
       <c r="Q96" t="inlineStr">
         <is>
-          <t>21/10/2023 08:01</t>
+          <t>21/10/2023 09:58</t>
         </is>
       </c>
       <c r="R96" t="n">
-        <v>3.54</v>
+        <v>1.83</v>
       </c>
       <c r="S96" t="inlineStr">
         <is>
@@ -9276,16 +9276,16 @@
         </is>
       </c>
       <c r="T96" t="n">
-        <v>3.9</v>
+        <v>1.68</v>
       </c>
       <c r="U96" t="inlineStr">
         <is>
-          <t>21/10/2023 06:21</t>
+          <t>21/10/2023 09:58</t>
         </is>
       </c>
       <c r="V96" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/romania/liga-2/csm-resita-tunari/2yBsKUlE/</t>
+          <t>https://www.betexplorer.com/football/romania/liga-2/progresul-spartac-metaloglobus-bucharest/nTSfdRd7/</t>
         </is>
       </c>
     </row>
@@ -9957,22 +9957,22 @@
       </c>
       <c r="F104" t="inlineStr">
         <is>
-          <t>Tunari</t>
+          <t>Selimbar</t>
         </is>
       </c>
       <c r="G104" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H104" t="inlineStr">
         <is>
-          <t>Viitorul Tg. Jiu</t>
+          <t>CSC Dumbravita</t>
         </is>
       </c>
       <c r="I104" t="n">
         <v>0</v>
       </c>
       <c r="J104" t="n">
-        <v>2.13</v>
+        <v>1.75</v>
       </c>
       <c r="K104" t="inlineStr">
         <is>
@@ -9980,15 +9980,15 @@
         </is>
       </c>
       <c r="L104" t="n">
-        <v>2.18</v>
+        <v>1.79</v>
       </c>
       <c r="M104" t="inlineStr">
         <is>
-          <t>28/10/2023 09:59</t>
+          <t>28/10/2023 09:51</t>
         </is>
       </c>
       <c r="N104" t="n">
-        <v>3.22</v>
+        <v>3.4</v>
       </c>
       <c r="O104" t="inlineStr">
         <is>
@@ -9996,15 +9996,15 @@
         </is>
       </c>
       <c r="P104" t="n">
-        <v>3.46</v>
+        <v>3.56</v>
       </c>
       <c r="Q104" t="inlineStr">
         <is>
-          <t>28/10/2023 09:59</t>
+          <t>28/10/2023 09:58</t>
         </is>
       </c>
       <c r="R104" t="n">
-        <v>3.11</v>
+        <v>4.23</v>
       </c>
       <c r="S104" t="inlineStr">
         <is>
@@ -10012,16 +10012,16 @@
         </is>
       </c>
       <c r="T104" t="n">
-        <v>3.24</v>
+        <v>4.62</v>
       </c>
       <c r="U104" t="inlineStr">
         <is>
-          <t>28/10/2023 09:59</t>
+          <t>28/10/2023 09:51</t>
         </is>
       </c>
       <c r="V104" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/romania/liga-2/tunari-viitorul-targu-jiu/CA0HDSRs/</t>
+          <t>https://www.betexplorer.com/football/romania/liga-2/selimbar-csc-dumbravita/dbnw94tD/</t>
         </is>
       </c>
     </row>
@@ -10049,7 +10049,7 @@
       </c>
       <c r="F105" t="inlineStr">
         <is>
-          <t>Selimbar</t>
+          <t>Mioveni</t>
         </is>
       </c>
       <c r="G105" t="n">
@@ -10057,14 +10057,14 @@
       </c>
       <c r="H105" t="inlineStr">
         <is>
-          <t>CSC Dumbravita</t>
+          <t>Concordia</t>
         </is>
       </c>
       <c r="I105" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J105" t="n">
-        <v>1.75</v>
+        <v>3.02</v>
       </c>
       <c r="K105" t="inlineStr">
         <is>
@@ -10072,15 +10072,15 @@
         </is>
       </c>
       <c r="L105" t="n">
-        <v>1.79</v>
+        <v>3.13</v>
       </c>
       <c r="M105" t="inlineStr">
         <is>
-          <t>28/10/2023 09:51</t>
+          <t>28/10/2023 09:52</t>
         </is>
       </c>
       <c r="N105" t="n">
-        <v>3.4</v>
+        <v>3.04</v>
       </c>
       <c r="O105" t="inlineStr">
         <is>
@@ -10088,15 +10088,15 @@
         </is>
       </c>
       <c r="P105" t="n">
-        <v>3.56</v>
+        <v>2.92</v>
       </c>
       <c r="Q105" t="inlineStr">
         <is>
-          <t>28/10/2023 09:58</t>
+          <t>28/10/2023 09:09</t>
         </is>
       </c>
       <c r="R105" t="n">
-        <v>4.23</v>
+        <v>2.27</v>
       </c>
       <c r="S105" t="inlineStr">
         <is>
@@ -10104,16 +10104,16 @@
         </is>
       </c>
       <c r="T105" t="n">
-        <v>4.62</v>
+        <v>2.53</v>
       </c>
       <c r="U105" t="inlineStr">
         <is>
-          <t>28/10/2023 09:51</t>
+          <t>28/10/2023 09:52</t>
         </is>
       </c>
       <c r="V105" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/romania/liga-2/selimbar-csc-dumbravita/dbnw94tD/</t>
+          <t>https://www.betexplorer.com/football/romania/liga-2/mioveni-concordia/A1EkI8JQ/</t>
         </is>
       </c>
     </row>
@@ -10233,22 +10233,22 @@
       </c>
       <c r="F107" t="inlineStr">
         <is>
-          <t>Mioveni</t>
+          <t>Tunari</t>
         </is>
       </c>
       <c r="G107" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H107" t="inlineStr">
         <is>
-          <t>Concordia</t>
+          <t>Viitorul Tg. Jiu</t>
         </is>
       </c>
       <c r="I107" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J107" t="n">
-        <v>3.02</v>
+        <v>2.13</v>
       </c>
       <c r="K107" t="inlineStr">
         <is>
@@ -10256,15 +10256,15 @@
         </is>
       </c>
       <c r="L107" t="n">
-        <v>3.13</v>
+        <v>2.18</v>
       </c>
       <c r="M107" t="inlineStr">
         <is>
-          <t>28/10/2023 09:52</t>
+          <t>28/10/2023 09:59</t>
         </is>
       </c>
       <c r="N107" t="n">
-        <v>3.04</v>
+        <v>3.22</v>
       </c>
       <c r="O107" t="inlineStr">
         <is>
@@ -10272,15 +10272,15 @@
         </is>
       </c>
       <c r="P107" t="n">
-        <v>2.92</v>
+        <v>3.46</v>
       </c>
       <c r="Q107" t="inlineStr">
         <is>
-          <t>28/10/2023 09:09</t>
+          <t>28/10/2023 09:59</t>
         </is>
       </c>
       <c r="R107" t="n">
-        <v>2.27</v>
+        <v>3.11</v>
       </c>
       <c r="S107" t="inlineStr">
         <is>
@@ -10288,16 +10288,16 @@
         </is>
       </c>
       <c r="T107" t="n">
-        <v>2.53</v>
+        <v>3.24</v>
       </c>
       <c r="U107" t="inlineStr">
         <is>
-          <t>28/10/2023 09:52</t>
+          <t>28/10/2023 09:59</t>
         </is>
       </c>
       <c r="V107" t="inlineStr">
         <is>
-          <t>https://www.betexplorer.com/football/romania/liga-2/mioveni-concordia/A1EkI8JQ/</t>
+          <t>https://www.betexplorer.com/football/romania/liga-2/tunari-viitorul-targu-jiu/CA0HDSRs/</t>
         </is>
       </c>
     </row>
@@ -11586,6 +11586,98 @@
       <c r="V121" t="inlineStr">
         <is>
           <t>https://www.betexplorer.com/football/romania/liga-2/unirea-slobozia-fc-buzau/Mqj1DJXb/</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" s="1" t="n">
+        <v>121</v>
+      </c>
+      <c r="B122" t="inlineStr">
+        <is>
+          <t>romania</t>
+        </is>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>liga-2</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>2023-2024</t>
+        </is>
+      </c>
+      <c r="E122" s="2" t="n">
+        <v>45239.77083333334</v>
+      </c>
+      <c r="F122" t="inlineStr">
+        <is>
+          <t>Chindia Targoviste</t>
+        </is>
+      </c>
+      <c r="G122" t="n">
+        <v>0</v>
+      </c>
+      <c r="H122" t="inlineStr">
+        <is>
+          <t>Mioveni</t>
+        </is>
+      </c>
+      <c r="I122" t="n">
+        <v>2</v>
+      </c>
+      <c r="J122" t="n">
+        <v>2.13</v>
+      </c>
+      <c r="K122" t="inlineStr">
+        <is>
+          <t>09/11/2023 08:15</t>
+        </is>
+      </c>
+      <c r="L122" t="n">
+        <v>1.83</v>
+      </c>
+      <c r="M122" t="inlineStr">
+        <is>
+          <t>09/11/2023 18:25</t>
+        </is>
+      </c>
+      <c r="N122" t="n">
+        <v>3.02</v>
+      </c>
+      <c r="O122" t="inlineStr">
+        <is>
+          <t>09/11/2023 08:15</t>
+        </is>
+      </c>
+      <c r="P122" t="n">
+        <v>3.23</v>
+      </c>
+      <c r="Q122" t="inlineStr">
+        <is>
+          <t>09/11/2023 18:25</t>
+        </is>
+      </c>
+      <c r="R122" t="n">
+        <v>3.79</v>
+      </c>
+      <c r="S122" t="inlineStr">
+        <is>
+          <t>09/11/2023 08:15</t>
+        </is>
+      </c>
+      <c r="T122" t="n">
+        <v>4.94</v>
+      </c>
+      <c r="U122" t="inlineStr">
+        <is>
+          <t>09/11/2023 18:28</t>
+        </is>
+      </c>
+      <c r="V122" t="inlineStr">
+        <is>
+          <t>https://www.betexplorer.com/football/romania/liga-2/chindia-targoviste-mioveni/AsGuA5r4/</t>
         </is>
       </c>
     </row>

</xml_diff>